<commit_message>
Update auf 2021 Daten - finales Update vor Repo Migration
</commit_message>
<xml_diff>
--- a/Tabelle_G8.xlsx
+++ b/Tabelle_G8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_projects\GISD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Git\GISD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8E11B45-FAD0-48FD-BB9C-0380E7A3A6EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE4573D-F681-4067-AE04-D70FED82327C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{26C7A7AC-2691-4E4A-821E-1A7F5D9D4762}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12230" xr2:uid="{26C7A7AC-2691-4E4A-821E-1A7F5D9D4762}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Jahr
 Einführung G8</t>
@@ -117,11 +117,14 @@
 Rücknahme G8 /Rückkehr G9</t>
   </si>
   <si>
-    <t>2026, 2027</t>
-  </si>
-  <si>
     <t>Quellen: https://www.kmk.org/themen/allgemeinbildende-schulen/bildungswege-und-abschluesse/sekundarstufe-ii-gymnasiale-oberstufe-und-abitur.html, 
 https://www.diw.de/de/diw_01.c.497179.de/publikationen/roundup/2015_0057/empirische_befunde_zu_auswirkungen_der_g8-schulzeitverkuerzung.html</t>
+  </si>
+  <si>
+    <t>Jahr mit weniger Abschlüssen</t>
+  </si>
+  <si>
+    <t>2025, 2026</t>
   </si>
 </sst>
 </file>
@@ -553,19 +556,19 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -579,10 +582,10 @@
         <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -596,10 +599,10 @@
         <v>23</v>
       </c>
       <c r="E2" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -613,10 +616,10 @@
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -633,7 +636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -650,7 +653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,7 +670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -684,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -697,11 +700,11 @@
       <c r="D8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="7">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -718,7 +721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -732,10 +735,10 @@
         <v>27</v>
       </c>
       <c r="E10" s="7">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -749,10 +752,10 @@
         <v>26</v>
       </c>
       <c r="E11" s="7">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -769,7 +772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -786,7 +789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -803,7 +806,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -820,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -834,10 +837,10 @@
         <v>2019</v>
       </c>
       <c r="E16" s="7">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -854,9 +857,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>

</xml_diff>